<commit_message>
novos testes para estudo do desempenho dos ajustes
</commit_message>
<xml_diff>
--- a/resultadosCompletosPerto.xlsx
+++ b/resultadosCompletosPerto.xlsx
@@ -452,10 +452,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22.02093756535208</v>
+        <v>5.350744530264296</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1000000000000014</v>
+        <v>0.1000000000000011</v>
       </c>
       <c r="C2" t="n">
         <v>0.1</v>

</xml_diff>